<commit_message>
Added new comparison for CD. More work on my thesis. Added Slides.
</commit_message>
<xml_diff>
--- a/DOCS/Theses/Ruocco/Latex/Giordano.xlsx
+++ b/DOCS/Theses/Ruocco/Latex/Giordano.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="113" windowWidth="23310" windowHeight="9983" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="113" windowWidth="23310" windowHeight="9983" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Giordano" sheetId="1" r:id="rId1"/>
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="56">
   <si>
     <t>AR</t>
   </si>
@@ -702,12 +702,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -715,6 +709,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Colore 1" xfId="2" builtinId="30"/>
@@ -724,6 +724,27 @@
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="66">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -785,33 +806,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -960,6 +954,12 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1078,11 +1078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198394368"/>
-        <c:axId val="171146560"/>
+        <c:axId val="143565312"/>
+        <c:axId val="143075008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198394368"/>
+        <c:axId val="143565312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1143,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171146560"/>
+        <c:crossAx val="143075008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1151,7 +1151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171146560"/>
+        <c:axId val="143075008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1162,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198394368"/>
+        <c:crossAx val="143565312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1499,11 +1499,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="148059648"/>
-        <c:axId val="140154496"/>
+        <c:axId val="146200064"/>
+        <c:axId val="146261696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148059648"/>
+        <c:axId val="146200064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1542,7 +1542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140154496"/>
+        <c:crossAx val="146261696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1550,7 +1550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140154496"/>
+        <c:axId val="146261696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148059648"/>
+        <c:crossAx val="146200064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1723,7 +1723,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Delft!$Q$7:$Q$26</c:f>
+              <c:f>Delft!$R$7:$R$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1879,11 +1879,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144143872"/>
-        <c:axId val="141890048"/>
+        <c:axId val="146202112"/>
+        <c:axId val="146263424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144143872"/>
+        <c:axId val="146202112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1943,7 +1943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141890048"/>
+        <c:crossAx val="146263424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1951,7 +1951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141890048"/>
+        <c:axId val="146263424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1962,7 +1962,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144143872"/>
+        <c:crossAx val="146202112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2095,11 +2095,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198394880"/>
-        <c:axId val="196813952"/>
+        <c:axId val="143565824"/>
+        <c:axId val="143073280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198394880"/>
+        <c:axId val="143565824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2135,7 +2135,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196813952"/>
+        <c:crossAx val="143073280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2143,7 +2143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196813952"/>
+        <c:axId val="143073280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +2154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198394880"/>
+        <c:crossAx val="143565824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2290,11 +2290,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198395392"/>
-        <c:axId val="196815680"/>
+        <c:axId val="143566336"/>
+        <c:axId val="143077312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198395392"/>
+        <c:axId val="143566336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2330,7 +2330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196815680"/>
+        <c:crossAx val="143077312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2338,7 +2338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196815680"/>
+        <c:axId val="143077312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2349,7 +2349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198395392"/>
+        <c:crossAx val="143566336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2482,11 +2482,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198395904"/>
-        <c:axId val="196817408"/>
+        <c:axId val="143566848"/>
+        <c:axId val="143079040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198395904"/>
+        <c:axId val="143566848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2546,7 +2546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196817408"/>
+        <c:crossAx val="143079040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2554,7 +2554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196817408"/>
+        <c:axId val="143079040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,7 +2565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198395904"/>
+        <c:crossAx val="143566848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2602,7 +2602,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2698,11 +2697,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="149456896"/>
-        <c:axId val="210538432"/>
+        <c:axId val="143567360"/>
+        <c:axId val="143080768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149456896"/>
+        <c:axId val="143567360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2711,7 +2710,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210538432"/>
+        <c:crossAx val="143080768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2719,7 +2718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210538432"/>
+        <c:axId val="143080768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2730,14 +2729,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149456896"/>
+        <c:crossAx val="143567360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2866,11 +2864,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="128502272"/>
-        <c:axId val="126348096"/>
+        <c:axId val="139107840"/>
+        <c:axId val="144960320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128502272"/>
+        <c:axId val="139107840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2879,7 +2877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126348096"/>
+        <c:crossAx val="144960320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2887,7 +2885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126348096"/>
+        <c:axId val="144960320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2898,7 +2896,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128502272"/>
+        <c:crossAx val="139107840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2952,7 +2950,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Delft!$Q$7:$Q$26</c:f>
+              <c:f>Delft!$R$7:$R$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -3031,11 +3029,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126536192"/>
-        <c:axId val="199804032"/>
+        <c:axId val="143567872"/>
+        <c:axId val="144961472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126536192"/>
+        <c:axId val="143567872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,7 +3042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199804032"/>
+        <c:crossAx val="144961472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3052,7 +3050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199804032"/>
+        <c:axId val="144961472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3063,7 +3061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126536192"/>
+        <c:crossAx val="143567872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3192,11 +3190,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126534144"/>
-        <c:axId val="8128768"/>
+        <c:axId val="146199040"/>
+        <c:axId val="144963776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126534144"/>
+        <c:axId val="146199040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3205,7 +3203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8128768"/>
+        <c:crossAx val="144963776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3213,7 +3211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8128768"/>
+        <c:axId val="144963776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3224,7 +3222,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126534144"/>
+        <c:crossAx val="146199040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3353,11 +3351,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="148474368"/>
-        <c:axId val="140150464"/>
+        <c:axId val="146200576"/>
+        <c:axId val="146259968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148474368"/>
+        <c:axId val="146200576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3366,7 +3364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140150464"/>
+        <c:crossAx val="146259968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3374,7 +3372,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140150464"/>
+        <c:axId val="146259968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3385,7 +3383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148474368"/>
+        <c:crossAx val="146200576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3782,7 +3780,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="AQ6:BA27" totalsRowShown="0" headerRowDxfId="15" headerRowCellStyle="20% - Colore 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="AQ6:BA27" totalsRowShown="0" headerRowDxfId="22" headerRowCellStyle="20% - Colore 1">
   <autoFilter ref="AQ6:BA27"/>
   <tableColumns count="11">
     <tableColumn id="1" name="m1">
@@ -3806,16 +3804,16 @@
     <tableColumn id="7" name="m4meno">
       <calculatedColumnFormula>Tabella9[[#This Row],[m4meno]]+(Tabella11[[#This Row],[m4meno]]-Tabella9[[#This Row],[m4meno]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Φ_1" dataDxfId="19">
+    <tableColumn id="8" name="Φ_1" dataDxfId="21">
       <calculatedColumnFormula>Tabella9[[#This Row],[Φ_1]]+(Tabella11[[#This Row],[Φ_1]]-Tabella9[[#This Row],[Φ_1]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Φ_2" dataDxfId="18">
+    <tableColumn id="9" name="Φ_2" dataDxfId="20">
       <calculatedColumnFormula>Tabella9[[#This Row],[Φ_2]]+(Tabella11[[#This Row],[Φ_2]]-Tabella9[[#This Row],[Φ_2]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Φ_3" dataDxfId="17">
+    <tableColumn id="10" name="Φ_3" dataDxfId="19">
       <calculatedColumnFormula>Tabella9[[#This Row],[Φ_3]]+(Tabella11[[#This Row],[Φ_3]]-Tabella9[[#This Row],[Φ_3]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Φ_4" dataDxfId="16">
+    <tableColumn id="11" name="Φ_4" dataDxfId="18">
       <calculatedColumnFormula>Tabella9[[#This Row],[Φ_4]]+(Tabella11[[#This Row],[Φ_4]]-Tabella9[[#This Row],[Φ_4]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3837,10 +3835,10 @@
     <tableColumn id="5" name="r = 1/λ"/>
     <tableColumn id="6" name="X0"/>
     <tableColumn id="7" name="m0"/>
-    <tableColumn id="8" name="d" dataDxfId="24">
+    <tableColumn id="8" name="d" dataDxfId="17">
       <calculatedColumnFormula xml:space="preserve"> SQRT(J2^2 + (I2-0.75*B2)^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="φ" dataDxfId="23">
+    <tableColumn id="9" name="φ" dataDxfId="16">
       <calculatedColumnFormula>ATAN((Tabella224[[#This Row],[m0]]/(Tabella224[[#This Row],[X0]]-0.75*Tabella224[[#This Row],[Cr]])))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3849,50 +3847,51 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabella24" displayName="Tabella24" ref="A6:Q27" totalsRowShown="0" headerRowCellStyle="Colore 1" dataCellStyle="Colore 1">
-  <autoFilter ref="A6:Q27"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabella24" displayName="Tabella24" ref="A6:R27" totalsRowShown="0" headerRowCellStyle="Colore 1" dataCellStyle="Colore 1">
+  <autoFilter ref="A6:R27"/>
+  <tableColumns count="18">
     <tableColumn id="1" name="α_abs">
       <calculatedColumnFormula>A6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="α_b" dataDxfId="22">
+    <tableColumn id="2" name="α_b" dataDxfId="15">
       <calculatedColumnFormula>Tabella3[[#This Row],[α_abs]]+Tabella224[α0_w]*57.3-Tabella224[iw]*57.3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="α_w" dataDxfId="21">
+    <tableColumn id="3" name="α_w" dataDxfId="14">
       <calculatedColumnFormula>Tabella3[[#This Row],[α_b]]+Tabella224[iw]*57.3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="CL_α"/>
     <tableColumn id="5" name="CL"/>
-    <tableColumn id="14" name="X" dataDxfId="14"/>
-    <tableColumn id="8" name="m" dataDxfId="20"/>
-    <tableColumn id="6" name="r (X/b/2)" dataDxfId="13">
+    <tableColumn id="14" name="X" dataDxfId="13"/>
+    <tableColumn id="8" name="m" dataDxfId="12"/>
+    <tableColumn id="6" name="r (X/b/2)" dataDxfId="11">
       <calculatedColumnFormula>Tabella24[[#This Row],[X]]/Tabella224[b/2]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="m (m/b/2)" dataDxfId="12">
+    <tableColumn id="7" name="m (m/b/2)" dataDxfId="10">
       <calculatedColumnFormula>Tabella24[[#This Row],[m]]/Tabella224[b/2]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Kε_Λ" dataDxfId="11">
+    <tableColumn id="11" name="Kε_Λ" dataDxfId="9">
       <calculatedColumnFormula>((0.1124 + 0.1265 * Tabella224[Λ_c/4] + 0.1766 * Tabella224[Λ_c/4]^2)/Tabella24[[#This Row],[r (X/b/2)]]^2) + (0.1024/Tabella24[[#This Row],[r (X/b/2)]]) +2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Kε_Λ0" dataDxfId="10">
+    <tableColumn id="9" name="Kε_Λ0" dataDxfId="8">
       <calculatedColumnFormula>(0.1124/Tabella24[[#This Row],[r (X/b/2)]]^2) + ( 0.1024/Tabella24[[#This Row],[r (X/b/2)]]) + 2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="dε/dα_k" dataDxfId="9">
+    <tableColumn id="13" name="dε/dα_k" dataDxfId="7">
       <calculatedColumnFormula>Tabella24[[#This Row],[Kε_Λ]]/Tabella24[[#This Row],[Kε_Λ0]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="dε/dα_1" dataDxfId="8" dataCellStyle="Normale">
+    <tableColumn id="10" name="dε/dα_1" dataDxfId="6" dataCellStyle="Normale">
       <calculatedColumnFormula>(Tabella24[[#This Row],[r (X/b/2)]]/(Tabella24[[#This Row],[r (X/b/2)]]^2 + Tabella24[[#This Row],[m (m/b/2)]]^2))* (0.4876/(SQRT(Tabella24[[#This Row],[r (X/b/2)]]^2 + 0.6319 + Tabella24[[#This Row],[m (m/b/2)]]^2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="dε/dα_2" dataDxfId="7" dataCellStyle="Normale">
+    <tableColumn id="12" name="dε/dα_2" dataDxfId="5" dataCellStyle="Normale">
       <calculatedColumnFormula>(1+(Tabella24[[#This Row],[r (X/b/2)]]^2/(Tabella24[[#This Row],[r (X/b/2)]]^2+0.7915 + 5.074 * Tabella24[[#This Row],[m (m/b/2)]]^2))^(0.3113))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="dε/dα_3" dataDxfId="6" dataCellStyle="Normale">
+    <tableColumn id="15" name="dε/dα_3" dataDxfId="4" dataCellStyle="Normale">
       <calculatedColumnFormula>(1-(SQRT((Tabella24[[#This Row],[m (m/b/2)]]^2)/(1+Tabella24[[#This Row],[m (m/b/2)]]^2))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="dε/dα" dataDxfId="5" dataCellStyle="Normale">
+    <tableColumn id="16" name="dε/dα" dataDxfId="3" dataCellStyle="Normale">
       <calculatedColumnFormula>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="ε" dataDxfId="4" dataCellStyle="Normale">
+    <tableColumn id="18" name="Colonna1"/>
+    <tableColumn id="17" name="ε" dataDxfId="2" dataCellStyle="Normale">
       <calculatedColumnFormula>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3950,19 +3949,19 @@
     <tableColumn id="9" name="m_P" dataDxfId="57">
       <calculatedColumnFormula>Tabella3[[#This Row],[m]]/Tabella2[b/2]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Φ" dataDxfId="2">
+    <tableColumn id="10" name="Φ" dataDxfId="56">
       <calculatedColumnFormula>Tabella14[[#This Row],[Φ_80]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="ε" dataDxfId="56">
+    <tableColumn id="11" name="ε" dataDxfId="55">
       <calculatedColumnFormula>Tabella3[[#This Row],[Φ]]*Tabella3[[#This Row],[CL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="dΦ/dα" dataDxfId="55">
+    <tableColumn id="12" name="dΦ/dα" dataDxfId="54">
       <calculatedColumnFormula>(J8-Tabella3[[#This Row],[Φ]])/(B8-Tabella3[[#This Row],[α_b]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="dε/dα" dataDxfId="54">
+    <tableColumn id="13" name="dε/dα" dataDxfId="53">
       <calculatedColumnFormula>Tabella3[[#This Row],[Φ]]*Tabella3[[#This Row],[CL_α]]+Tabella3[[#This Row],[CL]]*Tabella3[[#This Row],[dΦ/dα]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Colonna1" dataDxfId="3">
+    <tableColumn id="14" name="Colonna1" dataDxfId="52">
       <calculatedColumnFormula>Tabella3[[#This Row],[dε/dα]]*Tabella3[[#This Row],[α_abs]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4025,7 +4024,7 @@
     <tableColumn id="6" name="m3meno">
       <calculatedColumnFormula>AG7-10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="m4" dataDxfId="53">
+    <tableColumn id="7" name="m4" dataDxfId="51">
       <calculatedColumnFormula>Tabella11[[#This Row],[m3]]+10</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="m4meno">
@@ -4057,25 +4056,25 @@
   <autoFilter ref="Q35:AB56"/>
   <tableColumns count="12">
     <tableColumn id="1" name="mTab"/>
-    <tableColumn id="2" name="m1" dataDxfId="52">
+    <tableColumn id="2" name="m1" dataDxfId="50">
       <calculatedColumnFormula>E7*Tabella18[[#This Row],[mTab]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="m2" dataDxfId="51">
+    <tableColumn id="3" name="m2" dataDxfId="49">
       <calculatedColumnFormula>Tabella18[[#This Row],[m1]]+10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="m2meno" dataDxfId="50">
+    <tableColumn id="4" name="m2meno" dataDxfId="48">
       <calculatedColumnFormula>Tabella18[[#This Row],[m1]]-10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="m3" dataDxfId="49">
+    <tableColumn id="5" name="m3" dataDxfId="47">
       <calculatedColumnFormula>Tabella18[[#This Row],[m1]]+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="m3meno" dataDxfId="48">
+    <tableColumn id="6" name="m3meno" dataDxfId="46">
       <calculatedColumnFormula>Tabella18[[#This Row],[m2meno]]-10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="m4" dataDxfId="47">
+    <tableColumn id="7" name="m4" dataDxfId="45">
       <calculatedColumnFormula>Tabella18[[#This Row],[m1]]+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="m4meno" dataDxfId="46">
+    <tableColumn id="8" name="m4meno" dataDxfId="44">
       <calculatedColumnFormula>Tabella18[[#This Row],[m3meno]]-10</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="Φ_1"/>
@@ -4088,29 +4087,29 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tabella19" displayName="Tabella19" ref="AD35:AO56" totalsRowShown="0" headerRowDxfId="45" headerRowCellStyle="20% - Colore 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tabella19" displayName="Tabella19" ref="AD35:AO56" totalsRowShown="0" headerRowDxfId="43" headerRowCellStyle="20% - Colore 1">
   <autoFilter ref="AD35:AO56"/>
   <tableColumns count="12">
     <tableColumn id="1" name="mTab"/>
-    <tableColumn id="2" name="m1" dataDxfId="44">
+    <tableColumn id="2" name="m1" dataDxfId="42">
       <calculatedColumnFormula>Tabella19[[#This Row],[mTab]]*E7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="m2" dataDxfId="43">
+    <tableColumn id="3" name="m2" dataDxfId="41">
       <calculatedColumnFormula>Tabella19[[#This Row],[m1]]+10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="m2meno" dataDxfId="42">
+    <tableColumn id="4" name="m2meno" dataDxfId="40">
       <calculatedColumnFormula>Tabella19[[#This Row],[m1]]-10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="m3" dataDxfId="41">
+    <tableColumn id="5" name="m3" dataDxfId="39">
       <calculatedColumnFormula>Tabella19[[#This Row],[m2]]+10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="m3meno" dataDxfId="40">
+    <tableColumn id="6" name="m3meno" dataDxfId="38">
       <calculatedColumnFormula>Tabella19[[#This Row],[m2meno]]-10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="m4" dataDxfId="39">
+    <tableColumn id="7" name="m4" dataDxfId="37">
       <calculatedColumnFormula>Tabella19[[#This Row],[m3]]+10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="m4meno" dataDxfId="38">
+    <tableColumn id="8" name="m4meno" dataDxfId="36">
       <calculatedColumnFormula>Tabella19[[#This Row],[m3meno]]-10</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="Φ_1"/>
@@ -4123,40 +4122,40 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tabella21" displayName="Tabella21" ref="AQ35:BA55" totalsRowShown="0" headerRowDxfId="37" headerRowCellStyle="20% - Colore 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tabella21" displayName="Tabella21" ref="AQ35:BA55" totalsRowShown="0" headerRowDxfId="35" headerRowCellStyle="20% - Colore 1">
   <autoFilter ref="AQ35:BA55"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="m1" dataDxfId="36">
+    <tableColumn id="1" name="m1" dataDxfId="34">
       <calculatedColumnFormula>Tabella18[[#This Row],[m1]]+(Tabella19[[#This Row],[m1]]-Tabella18[[#This Row],[m1]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="m2" dataDxfId="35">
+    <tableColumn id="2" name="m2" dataDxfId="33">
       <calculatedColumnFormula>Tabella18[[#This Row],[m2]]+(Tabella19[[#This Row],[m2]]-Tabella18[[#This Row],[m2]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="m2meno" dataDxfId="34">
+    <tableColumn id="3" name="m2meno" dataDxfId="32">
       <calculatedColumnFormula>Tabella18[[#This Row],[m2meno]]+(Tabella19[[#This Row],[m2meno]]-Tabella18[[#This Row],[m2meno]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="m3" dataDxfId="33">
+    <tableColumn id="4" name="m3" dataDxfId="31">
       <calculatedColumnFormula>Tabella18[[#This Row],[m3]]+(Tabella19[[#This Row],[m3]]-Tabella18[[#This Row],[m3]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="m3meno" dataDxfId="32">
+    <tableColumn id="5" name="m3meno" dataDxfId="30">
       <calculatedColumnFormula>Tabella18[[#This Row],[m3meno]]+(Tabella19[[#This Row],[m3meno]]-Tabella18[[#This Row],[m3meno]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="m4" dataDxfId="31">
+    <tableColumn id="6" name="m4" dataDxfId="29">
       <calculatedColumnFormula>Tabella18[[#This Row],[m4]]+(Tabella19[[#This Row],[m4]]-Tabella18[[#This Row],[m4]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="m4meno" dataDxfId="30">
+    <tableColumn id="7" name="m4meno" dataDxfId="28">
       <calculatedColumnFormula>Tabella18[[#This Row],[m4meno]]+(Tabella19[[#This Row],[m4meno]]-Tabella18[[#This Row],[m4meno]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Φ_1" dataDxfId="29">
+    <tableColumn id="8" name="Φ_1" dataDxfId="27">
       <calculatedColumnFormula>Tabella18[[#This Row],[Φ_1]]+(Tabella19[[#This Row],[Φ_1]]-Tabella18[[#This Row],[Φ_1]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Φ_2" dataDxfId="28">
+    <tableColumn id="9" name="Φ_2" dataDxfId="26">
       <calculatedColumnFormula>Tabella18[[#This Row],[Φ_2]]+(Tabella19[[#This Row],[Φ_2]]-Tabella18[[#This Row],[Φ_2]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Φ_3" dataDxfId="27">
+    <tableColumn id="10" name="Φ_3" dataDxfId="25">
       <calculatedColumnFormula>Tabella18[[#This Row],[Φ_3]]+(Tabella19[[#This Row],[Φ_3]]-Tabella18[[#This Row],[Φ_3]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Φ_4" dataDxfId="26">
+    <tableColumn id="11" name="Φ_4" dataDxfId="24">
       <calculatedColumnFormula>Tabella18[[#This Row],[Φ_4]]+(Tabella19[[#This Row],[Φ_4]]-Tabella18[[#This Row],[Φ_4]])*((Tabella2[r = 1/λ]-1)/(2-1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4168,7 +4167,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tabella22" displayName="Tabella22" ref="BC35:BC55" totalsRowShown="0">
   <autoFilter ref="BC35:BC55"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Φ_90" dataDxfId="25">
+    <tableColumn id="1" name="Φ_90" dataDxfId="23">
       <calculatedColumnFormula>Tabella21[[#This Row],[Φ_3]]+(Tabella21[[#This Row],[Φ_4]]-Tabella21[[#This Row],[Φ_3]])*(I7-Tabella21[[#This Row],[m3]])/(Tabella21[[#This Row],[m4]]-Tabella21[[#This Row],[m3]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4465,8 +4464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC56"/>
   <sheetViews>
-    <sheetView topLeftCell="K13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4556,87 +4555,87 @@
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="Q4" s="9" t="s">
+      <c r="Q4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="9"/>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="9"/>
-      <c r="AT4" s="9"/>
-      <c r="AU4" s="9"/>
-      <c r="AV4" s="9"/>
-      <c r="AW4" s="9"/>
-      <c r="AX4" s="9"/>
-      <c r="AY4" s="9"/>
-      <c r="AZ4" s="9"/>
-      <c r="BA4" s="9"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="16"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="16"/>
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16"/>
+      <c r="AQ4" s="16"/>
+      <c r="AR4" s="16"/>
+      <c r="AS4" s="16"/>
+      <c r="AT4" s="16"/>
+      <c r="AU4" s="16"/>
+      <c r="AV4" s="16"/>
+      <c r="AW4" s="16"/>
+      <c r="AX4" s="16"/>
+      <c r="AY4" s="16"/>
+      <c r="AZ4" s="16"/>
+      <c r="BA4" s="16"/>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="R5" s="10" t="s">
+      <c r="R5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
-      <c r="AD5" s="10" t="s">
+      <c r="AD5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="10"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="10"/>
-      <c r="AL5" s="10"/>
-      <c r="AM5" s="10"/>
-      <c r="AN5" s="10"/>
-      <c r="AO5" s="10"/>
-      <c r="AQ5" s="10" t="s">
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="17"/>
+      <c r="AM5" s="17"/>
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="17"/>
+      <c r="AQ5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AR5" s="10"/>
-      <c r="AS5" s="10"/>
-      <c r="AT5" s="10"/>
-      <c r="AU5" s="10"/>
-      <c r="AV5" s="10"/>
-      <c r="AW5" s="10"/>
-      <c r="AX5" s="10"/>
-      <c r="AY5" s="10"/>
-      <c r="AZ5" s="10"/>
-      <c r="BA5" s="10"/>
+      <c r="AR5" s="17"/>
+      <c r="AS5" s="17"/>
+      <c r="AT5" s="17"/>
+      <c r="AU5" s="17"/>
+      <c r="AV5" s="17"/>
+      <c r="AW5" s="17"/>
+      <c r="AX5" s="17"/>
+      <c r="AY5" s="17"/>
+      <c r="AZ5" s="17"/>
+      <c r="BA5" s="17"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -8621,87 +8620,87 @@
       </c>
     </row>
     <row r="33" spans="17:55" x14ac:dyDescent="0.45">
-      <c r="Q33" s="9" t="s">
+      <c r="Q33" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
-      <c r="AA33" s="9"/>
-      <c r="AB33" s="9"/>
-      <c r="AC33" s="9"/>
-      <c r="AD33" s="9"/>
-      <c r="AE33" s="9"/>
-      <c r="AF33" s="9"/>
-      <c r="AG33" s="9"/>
-      <c r="AH33" s="9"/>
-      <c r="AI33" s="9"/>
-      <c r="AJ33" s="9"/>
-      <c r="AK33" s="9"/>
-      <c r="AL33" s="9"/>
-      <c r="AM33" s="9"/>
-      <c r="AN33" s="9"/>
-      <c r="AO33" s="9"/>
-      <c r="AP33" s="9"/>
-      <c r="AQ33" s="9"/>
-      <c r="AR33" s="9"/>
-      <c r="AS33" s="9"/>
-      <c r="AT33" s="9"/>
-      <c r="AU33" s="9"/>
-      <c r="AV33" s="9"/>
-      <c r="AW33" s="9"/>
-      <c r="AX33" s="9"/>
-      <c r="AY33" s="9"/>
-      <c r="AZ33" s="9"/>
-      <c r="BA33" s="9"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="16"/>
+      <c r="AB33" s="16"/>
+      <c r="AC33" s="16"/>
+      <c r="AD33" s="16"/>
+      <c r="AE33" s="16"/>
+      <c r="AF33" s="16"/>
+      <c r="AG33" s="16"/>
+      <c r="AH33" s="16"/>
+      <c r="AI33" s="16"/>
+      <c r="AJ33" s="16"/>
+      <c r="AK33" s="16"/>
+      <c r="AL33" s="16"/>
+      <c r="AM33" s="16"/>
+      <c r="AN33" s="16"/>
+      <c r="AO33" s="16"/>
+      <c r="AP33" s="16"/>
+      <c r="AQ33" s="16"/>
+      <c r="AR33" s="16"/>
+      <c r="AS33" s="16"/>
+      <c r="AT33" s="16"/>
+      <c r="AU33" s="16"/>
+      <c r="AV33" s="16"/>
+      <c r="AW33" s="16"/>
+      <c r="AX33" s="16"/>
+      <c r="AY33" s="16"/>
+      <c r="AZ33" s="16"/>
+      <c r="BA33" s="16"/>
     </row>
     <row r="34" spans="17:55" x14ac:dyDescent="0.45">
-      <c r="R34" s="10" t="s">
+      <c r="R34" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="10"/>
-      <c r="V34" s="10"/>
-      <c r="W34" s="10"/>
-      <c r="X34" s="10"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
       <c r="Y34" s="6"/>
       <c r="Z34" s="6"/>
       <c r="AA34" s="6"/>
       <c r="AB34" s="6"/>
-      <c r="AD34" s="10" t="s">
+      <c r="AD34" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="AE34" s="10"/>
-      <c r="AF34" s="10"/>
-      <c r="AG34" s="10"/>
-      <c r="AH34" s="10"/>
-      <c r="AI34" s="10"/>
-      <c r="AJ34" s="10"/>
-      <c r="AK34" s="10"/>
-      <c r="AL34" s="10"/>
-      <c r="AM34" s="10"/>
-      <c r="AN34" s="10"/>
-      <c r="AO34" s="10"/>
-      <c r="AQ34" s="10" t="s">
+      <c r="AE34" s="17"/>
+      <c r="AF34" s="17"/>
+      <c r="AG34" s="17"/>
+      <c r="AH34" s="17"/>
+      <c r="AI34" s="17"/>
+      <c r="AJ34" s="17"/>
+      <c r="AK34" s="17"/>
+      <c r="AL34" s="17"/>
+      <c r="AM34" s="17"/>
+      <c r="AN34" s="17"/>
+      <c r="AO34" s="17"/>
+      <c r="AQ34" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AR34" s="10"/>
-      <c r="AS34" s="10"/>
-      <c r="AT34" s="10"/>
-      <c r="AU34" s="10"/>
-      <c r="AV34" s="10"/>
-      <c r="AW34" s="10"/>
-      <c r="AX34" s="10"/>
-      <c r="AY34" s="10"/>
-      <c r="AZ34" s="10"/>
-      <c r="BA34" s="10"/>
+      <c r="AR34" s="17"/>
+      <c r="AS34" s="17"/>
+      <c r="AT34" s="17"/>
+      <c r="AU34" s="17"/>
+      <c r="AV34" s="17"/>
+      <c r="AW34" s="17"/>
+      <c r="AX34" s="17"/>
+      <c r="AY34" s="17"/>
+      <c r="AZ34" s="17"/>
+      <c r="BA34" s="17"/>
     </row>
     <row r="35" spans="17:55" x14ac:dyDescent="0.45">
       <c r="Q35" s="7" t="s">
@@ -11529,10 +11528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11544,10 +11543,10 @@
     <col min="13" max="13" width="12.6640625" customWidth="1"/>
     <col min="14" max="14" width="11.46484375" customWidth="1"/>
     <col min="15" max="15" width="11.9296875" customWidth="1"/>
-    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="16" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11585,7 +11584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>12</v>
       </c>
@@ -11625,7 +11624,7 @@
         <v>0.3318971510674355</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -11675,10 +11674,13 @@
         <v>21</v>
       </c>
       <c r="Q6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>0</v>
       </c>
@@ -11738,12 +11740,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.23438014029411439</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8">
         <f>A7+1</f>
         <v>1</v>
@@ -11804,12 +11806,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.23769520799969651</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>0.23769520799969651</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9">
         <f t="shared" ref="A9:A24" si="0">A8+1</f>
         <v>2</v>
@@ -11870,12 +11872,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.24101781007506587</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>0.48203562015013174</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -11936,12 +11938,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.24434543801554956</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>0.73303631404664871</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -12002,12 +12004,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.24767557364722045</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>0.99070229458888182</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -12068,12 +12070,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.25100570085486645</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>1.2550285042743323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -12134,12 +12136,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.25433331691224792</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>1.5259999014734875</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -12200,12 +12202,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.25765594330296093</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>1.8035916031207266</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -12266,12 +12268,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.26095978436525669</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>2.0876782749220535</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -12332,12 +12334,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.26410867011755362</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>2.3769780310579827</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -12398,12 +12400,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.26788806944964777</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>2.6788806944964776</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -12464,12 +12466,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.27505694766978228</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>3.025626424367605</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -12530,12 +12532,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.27999848151476864</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>3.3599817781772234</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -12596,12 +12598,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.27308717441307639</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>3.550133267369993</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -12662,12 +12664,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.25338620614989016</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>3.5474068860984622</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -12728,12 +12730,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.219456662906066</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>3.2918499435909898</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -12794,12 +12796,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>0.16913087654917869</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>2.706094024786859</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -12860,12 +12862,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>9.6195689958012046E-2</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>1.6353267292862048</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A25">
         <f>A24+1</f>
         <v>18</v>
@@ -12926,12 +12928,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>5.3749809662669195E-3</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>9.6749657392804556E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A26">
         <f t="shared" ref="A26:A27" si="1">A25+1</f>
         <v>19</v>
@@ -12992,12 +12994,12 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>-9.9560999519654567E-2</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>-1.8916589908734367</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -13058,7 +13060,7 @@
         <f>Tabella24[[#This Row],[dε/dα_k]]*(Tabella24[[#This Row],[dε/dα_1]]+Tabella24[[#This Row],[dε/dα_2]]*Tabella24[[#This Row],[dε/dα_3]])*(Tabella24[[#This Row],[CL_α]]*57.3/(3.14*Tabella224[AR]))</f>
         <v>-0.18759250970670097</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <f>Tabella24[[#This Row],[dε/dα]]*Tabella24[[#This Row],[α_abs]]</f>
         <v>-3.7518501941340192</v>
       </c>
@@ -13078,7 +13080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
@@ -13168,83 +13170,83 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <v>0</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <f>A6+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>-2.6684609999999997</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <f>B6+Tabella2245[iw]*57.3</f>
         <v>-1.1672009999999997</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>9.8282834347781997E-2</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>0.115402510819653</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>13.6917312039044</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <v>4.3124999907486403</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <v>0.08</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="10">
         <f>(1-(G6/(Tabella2245[b/2]*2)))/(((F6/Tabella2245[b/2]))^(1/3))</f>
         <v>0.83730887078770322</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="10">
         <f>4.44*(H6*I6*J6* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.21141554710975663</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="10">
         <f>A6*K6</f>
         <v>0</v>
       </c>
@@ -13254,46 +13256,46 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="13">
+      <c r="A7" s="11">
         <f>A6+1</f>
         <v>1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <f>A7+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>-1.668461</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <f>B7+Tabella2245[iw]*57.3</f>
         <v>-0.16720099999999993</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>9.8282834347781997E-2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="13">
         <v>0.21368534516743501</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="13">
         <v>13.745889410382899</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="12">
         <v>4.1566379898647403</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <v>0.08</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="10">
         <f>(1-(G7/(Tabella2245[b/2]*2)))/(((F7/Tabella2245[b/2]))^(1/3))</f>
         <v>0.84193732331697446</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="10">
         <f>4.44*(H7*I7*J7* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.21280697809328983</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="10">
         <f t="shared" ref="L7:L26" si="0">A7*K7</f>
         <v>0.21280697809328983</v>
       </c>
@@ -13303,856 +13305,856 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <f t="shared" ref="A8:A23" si="1">A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <f>A8+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>-0.66846099999999997</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <f>B8+Tabella2245[iw]*57.3</f>
         <v>0.83279900000000007</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>9.8282834347781997E-2</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>0.31196817951521699</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>13.797222731719399</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <v>4.0014437301949703</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>0.08</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="10">
         <f>(1-(G8/(Tabella2245[b/2]*2)))/(((F8/Tabella2245[b/2]))^(1/3))</f>
         <v>0.84658979064039164</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="10">
         <f>4.44*(H8*I8*J8* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.2142070939819975</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="10">
         <f t="shared" si="0"/>
         <v>0.428414187963995</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A9" s="13">
+      <c r="A9" s="11">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <f>A9+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>0.33153900000000003</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="10">
         <f>B9+Tabella2245[iw]*57.3</f>
         <v>1.8327990000000001</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>9.8282834347781997E-2</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="12">
         <v>0.410251013862999</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="12">
         <v>13.8457845025516</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="12">
         <v>3.8469638352084101</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <v>0.08</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="10">
         <f>(1-(G9/(Tabella2245[b/2]*2)))/(((F9/Tabella2245[b/2]))^(1/3))</f>
         <v>0.85126393048195292</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="10">
         <f>4.44*(H9*I9*J9* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.21561520494021139</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="10">
         <f t="shared" si="0"/>
         <v>0.64684561482063418</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" s="11">
+      <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <f>A10+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>1.331539</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <f>B10+Tabella2245[iw]*57.3</f>
         <v>2.8327990000000001</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <v>9.8282834347781997E-2</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>0.50853384821078196</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <v>13.8916290583707</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="10">
         <v>3.6932413891250002</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <v>0.08</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="10">
         <f>(1-(G10/(Tabella2245[b/2]*2)))/(((F10/Tabella2245[b/2]))^(1/3))</f>
         <v>0.85595753500617189</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="10">
         <f>4.44*(H10*I10*J10* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.21703065872248389</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="10">
         <f t="shared" si="0"/>
         <v>0.86812263488993557</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A11" s="13">
+      <c r="A11" s="11">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <f>A11+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>2.3315390000000003</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <f>B11+Tabella2245[iw]*57.3</f>
         <v>3.8327990000000005</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>9.8282834347781997E-2</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="12">
         <v>0.60681668255856303</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="12">
         <v>13.934811533044799</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="12">
         <v>3.54031591967399</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <v>0.08</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="10">
         <f>(1-(G11/(Tabella2245[b/2]*2)))/(((F11/Tabella2245[b/2]))^(1/3))</f>
         <v>0.86066853130470378</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="10">
         <f>4.44*(H11*I11*J11* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.21845284103266394</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="10">
         <f t="shared" si="0"/>
         <v>1.0922642051633198</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A12" s="11">
+      <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <f>A12+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>3.3315389999999994</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="10">
         <f>B12+Tabella2245[iw]*57.3</f>
         <v>4.8327989999999996</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="10">
         <v>9.8282834347779194E-2</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <v>0.70509951690631101</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <v>13.9753876574768</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="10">
         <v>3.3882234021856799</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="10">
         <v>0.08</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="10">
         <f>(1-(G12/(Tabella2245[b/2]*2)))/(((F12/Tabella2245[b/2]))^(1/3))</f>
         <v>0.86539498140749371</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="10">
         <f>4.44*(H12*I12*J12* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.21988117574318772</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="10">
         <f t="shared" si="0"/>
         <v>1.3192870544591262</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="13">
+      <c r="A13" s="11">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <f>A13+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>4.3315389999999994</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="10">
         <f>B13+Tabella2245[iw]*57.3</f>
         <v>5.8327989999999996</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <v>9.8282834347227094E-2</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="12">
         <v>0.80338235124850899</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="12">
         <v>14.0134135612502</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="12">
         <v>3.2369962841600901</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="10">
         <v>0.08</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="10">
         <f>(1-(G13/(Tabella2245[b/2]*2)))/(((F13/Tabella2245[b/2]))^(1/3))</f>
         <v>0.87013508181158605</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="10">
         <f>4.44*(H13*I13*J13* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.22131512497069225</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="10">
         <f t="shared" si="0"/>
         <v>1.5492058747948458</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="11">
+      <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <f>A14+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>5.3315389999999994</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="10">
         <f>B14+Tabella2245[iw]*57.3</f>
         <v>6.8327989999999996</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <v>9.8282834239803205E-2</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <v>0.90166518473535795</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <v>14.0488295971388</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="10">
         <v>3.0871771656852101</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="10">
         <v>0.08</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="10">
         <f>(1-(G14/(Tabella2245[b/2]*2)))/(((F14/Tabella2245[b/2]))^(1/3))</f>
         <v>0.87487082531166904</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="10">
         <f>4.44*(H14*I14*J14* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.22274923908738847</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="10">
         <f t="shared" si="0"/>
         <v>1.7819939126991078</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="13">
+      <c r="A15" s="11">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="10">
         <f>A15+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>6.3315389999999994</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="10">
         <f>B15+Tabella2245[iw]*57.3</f>
         <v>7.8327989999999996</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <v>9.8282813863925997E-2</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="12">
         <v>0.99994789521852601</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="12">
         <v>14.0804149076745</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="12">
         <v>2.9448243312074101</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <v>0.08</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="10">
         <f>(1-(G15/(Tabella2245[b/2]*2)))/(((F15/Tabella2245[b/2]))^(1/3))</f>
         <v>0.87940733916781999</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="10">
         <f>4.44*(H15*I15*J15* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.22412440495347286</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="10">
         <f t="shared" si="0"/>
         <v>2.0171196445812556</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A16" s="11">
+      <c r="A16" s="9">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="10">
         <f>A16+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>7.3315389999999994</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="10">
         <f>B16+Tabella2245[iw]*57.3</f>
         <v>8.8327989999999996</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="10">
         <v>9.8279039539641996E-2</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="10">
         <v>1.0984346730599399</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="10">
         <v>14.1156952451298</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="10">
         <v>2.77397755795876</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="10">
         <v>0.08</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="10">
         <f>(1-(G16/(Tabella2245[b/2]*2)))/(((F16/Tabella2245[b/2]))^(1/3))</f>
         <v>0.88489914221861798</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="10">
         <f>4.44*(H16*I16*J16* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.2257909540841605</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="10">
         <f t="shared" si="0"/>
         <v>2.257909540841605</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="13">
+      <c r="A17" s="11">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="10">
         <f>A17+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>8.3315389999999994</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="10">
         <f>B17+Tabella2245[iw]*57.3</f>
         <v>9.8327989999999996</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="12">
         <v>9.9188004814052794E-2</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="12">
         <v>1.19784355761298</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="12">
         <v>14.1549967368558</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="12">
         <v>2.56495212438475</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="10">
         <v>0.08</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="10">
         <f>(1-(G17/(Tabella2245[b/2]*2)))/(((F17/Tabella2245[b/2]))^(1/3))</f>
         <v>0.89168851861220011</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="10">
         <f>4.44*(H17*I17*J17* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.22785398337878934</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="10">
         <f t="shared" si="0"/>
         <v>2.5063938171666829</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="11">
+      <c r="A18" s="9">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="10">
         <f>A18+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>9.3315389999999994</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="10">
         <f>B18+Tabella2245[iw]*57.3</f>
         <v>10.832799</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="10">
         <v>9.8887374946945397E-2</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="10">
         <v>1.29450022632146</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="10">
         <v>14.1976370788321</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="10">
         <v>2.3073371737589401</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="10">
         <v>0.08</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="10">
         <f>(1-(G18/(Tabella2245[b/2]*2)))/(((F18/Tabella2245[b/2]))^(1/3))</f>
         <v>0.90016345171049772</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="10">
         <f>4.44*(H18*I18*J18* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.23043337713057238</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="10">
         <f t="shared" si="0"/>
         <v>2.7652005255668684</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="13">
+      <c r="A19" s="11">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="10">
         <f>A19+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>10.331538999999999</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="10">
         <f>B19+Tabella2245[iw]*57.3</f>
         <v>11.832799</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="12">
         <v>9.4047767782505606E-2</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="12">
         <v>1.38385770413853</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="12">
         <v>14.241623411473</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="12">
         <v>1.9888920790517799</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="10">
         <v>0.08</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="10">
         <f>(1-(G19/(Tabella2245[b/2]*2)))/(((F19/Tabella2245[b/2]))^(1/3))</f>
         <v>0.91080449878771463</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="10">
         <f>4.44*(H19*I19*J19* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.23367857539408221</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="10">
         <f t="shared" si="0"/>
         <v>3.0378214801230685</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="11">
+      <c r="A20" s="9">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="10">
         <f>A20+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>11.331538999999999</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="10">
         <f>B20+Tabella2245[iw]*57.3</f>
         <v>12.832799</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="10">
         <v>8.4661245764850707E-2</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="10">
         <v>1.4613690340788399</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="10">
         <v>14.282923617969701</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="10">
         <v>1.59433050140411</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="10">
         <v>0.08</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="10">
         <f>(1-(G20/(Tabella2245[b/2]*2)))/(((F20/Tabella2245[b/2]))^(1/3))</f>
         <v>0.92424590222758451</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="10">
         <f>4.44*(H20*I20*J20* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.2377880977557085</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="10">
         <f t="shared" si="0"/>
         <v>3.3290333685799189</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="13">
+      <c r="A21" s="11">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="10">
         <f>A21+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>12.331538999999999</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="10">
         <f>B21+Tabella2245[iw]*57.3</f>
         <v>13.832799</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="12">
         <v>7.0727767035164896E-2</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="12">
         <v>1.52248725921424</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="12">
         <v>14.3141548321128</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="12">
         <v>1.1042071248401699</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="10">
         <v>0.08</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="10">
         <f>(1-(G21/(Tabella2245[b/2]*2)))/(((F21/Tabella2245[b/2]))^(1/3))</f>
         <v>0.94134871974877865</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="10">
         <f>4.44*(H21*I21*J21* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.24303346885342084</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="10">
         <f t="shared" si="0"/>
         <v>3.6455020328013124</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="11">
+      <c r="A22" s="9">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="10">
         <f>A22+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>13.331538999999999</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="10">
         <f>B22+Tabella2245[iw]*57.3</f>
         <v>14.832799</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="10">
         <v>5.22473313753695E-2</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="10">
         <v>1.5626654226636201</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="10">
         <v>14.322331931719701</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="10">
         <v>0.49356996853757601</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="10">
         <v>0.08</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="10">
         <f>(1-(G22/(Tabella2245[b/2]*2)))/(((F22/Tabella2245[b/2]))^(1/3))</f>
         <v>0.96331153351232401</v>
       </c>
-      <c r="K22" s="12">
+      <c r="K22" s="10">
         <f>4.44*(H22*I22*J22* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.24979594951221692</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="10">
         <f t="shared" si="0"/>
         <v>3.9967351921954708</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="10">
         <f>A23+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>14.331538999999999</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="10">
         <f>B23+Tabella2245[iw]*57.3</f>
         <v>15.832799</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <v>2.92199383809684E-2</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="12">
         <v>1.57735657790398</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="12">
         <v>14.2872889124111</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="12">
         <v>-0.24306371705337901</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="10">
         <v>0.08</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="10">
         <f>(1-(G23/(Tabella2245[b/2]*2)))/(((F23/Tabella2245[b/2]))^(1/3))</f>
         <v>0.99083098716491791</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="10">
         <f>4.44*(H23*I23*J23* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.25831073071076377</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="10">
         <f t="shared" si="0"/>
         <v>4.391282422082984</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="11">
+      <c r="A24" s="9">
         <f>A23+1</f>
         <v>18</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="10">
         <f>A24+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>15.331539000000001</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="10">
         <f>B24+Tabella2245[iw]*57.3</f>
         <v>16.832799000000001</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="10">
         <v>1.6455383118552101E-3</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="10">
         <v>1.5620159470931601</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="10">
         <v>14.277065867523399</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="10">
         <v>-0.36563982436565901</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="10">
         <v>0.08</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="10">
         <f>(1-(G24/(Tabella2245[b/2]*2)))/(((F24/Tabella2245[b/2]))^(1/3))</f>
         <v>0.99551678547335065</v>
       </c>
-      <c r="K24" s="12">
+      <c r="K24" s="10">
         <f>4.44*(H24*I24*J24* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.25976507839472718</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="10">
         <f t="shared" si="0"/>
         <v>4.6757714111050888</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="13">
+      <c r="A25" s="11">
         <f t="shared" ref="A25:A26" si="2">A24+1</f>
         <v>19</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="10">
         <f>A25+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>16.331539000000003</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="10">
         <f>B25+Tabella2245[iw]*57.3</f>
         <v>17.832799000000001</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="12">
         <v>-3.0480375670981299E-2</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="12">
         <v>1.52305821961917</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="12">
         <v>14.277065867523399</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="12">
         <v>-0.36563982436565901</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="10">
         <v>0.08</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I25" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J25" s="12">
+      <c r="J25" s="10">
         <f>(1-(G25/(Tabella2245[b/2]*2)))/(((F25/Tabella2245[b/2]))^(1/3))</f>
         <v>0.99551678547335065</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K25" s="10">
         <f>4.44*(H25*I25*J25* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.25976507839472718</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="10">
         <f t="shared" si="0"/>
         <v>4.9355364894998166</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="11">
+      <c r="A26" s="9">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="10">
         <f>A26+Tabella2245[α0_w]*57.3 - Tabella2245[iw]*57.3</f>
         <v>17.331539000000003</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="10">
         <f>B26+Tabella2245[iw]*57.3</f>
         <v>18.832799000000001</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="10">
         <v>-5.7431024161159298E-2</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="10">
         <v>1.52305821961917</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="10">
         <v>14.277065867523399</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="10">
         <v>-0.36563982436565901</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="10">
         <v>0.08</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="10">
         <f>(10-3*Tabella2245[λ])/7</f>
         <v>1.1560000000000001</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="10">
         <f>(1-(G26/(Tabella2245[b/2]*2)))/(((F26/Tabella2245[b/2]))^(1/3))</f>
         <v>0.99551678547335065</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="10">
         <f>4.44*(H26*I26*J26* SQRT(COS(Tabella2245[Λ_c/4])))^(1.19)</f>
         <v>0.25976507839472718</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="10">
         <f t="shared" si="0"/>
         <v>5.1953015678945436</v>
       </c>

</xml_diff>